<commit_message>
update to customer sheet
</commit_message>
<xml_diff>
--- a/Data/cic_reports.xlsx
+++ b/Data/cic_reports.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UEL\RPA\RPA_CreditCardApproval\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89080F94-BE7C-49F6-8FCE-81FEFEA2FAF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C5FD616-68FE-41CC-B584-673EE1AF2D5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="52">
   <si>
     <t>cif</t>
   </si>
@@ -49,12 +49,6 @@
     <t>score_band</t>
   </si>
   <si>
-    <t>offer_limit</t>
-  </si>
-  <si>
-    <t>status</t>
-  </si>
-  <si>
     <t>CIC123802</t>
   </si>
   <si>
@@ -182,18 +176,6 @@
   </si>
   <si>
     <t>18/09/2004</t>
-  </si>
-  <si>
-    <t>Approved</t>
-  </si>
-  <si>
-    <t>Rejected</t>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t>No email</t>
   </si>
 </sst>
 </file>
@@ -231,7 +213,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -254,28 +236,16 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -579,19 +549,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K12"/>
+  <dimension ref="A1:I12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="L11" sqref="L11"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="119" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="M7" sqref="M7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="7" width="21.77734375" customWidth="1"/>
-    <col min="10" max="10" width="13.6640625" customWidth="1"/>
+    <col min="8" max="9" width="9.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -619,31 +589,25 @@
       <c r="I1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="2" t="s">
+    </row>
+    <row r="2" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
         <v>9</v>
-      </c>
-      <c r="K1" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>11</v>
       </c>
       <c r="B2">
         <v>33301007320</v>
       </c>
       <c r="C2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" t="s">
         <v>12</v>
       </c>
-      <c r="D2" t="s">
+      <c r="F2" t="s">
         <v>13</v>
-      </c>
-      <c r="E2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F2" t="s">
-        <v>15</v>
       </c>
       <c r="G2">
         <v>0</v>
@@ -652,33 +616,27 @@
         <v>746</v>
       </c>
       <c r="I2" t="s">
-        <v>16</v>
-      </c>
-      <c r="J2">
-        <v>6160000</v>
-      </c>
-      <c r="K2" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B3">
         <v>89854219200</v>
       </c>
       <c r="C3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E3" t="s">
         <v>18</v>
       </c>
-      <c r="D3" t="s">
+      <c r="F3" t="s">
         <v>19</v>
-      </c>
-      <c r="E3" t="s">
-        <v>20</v>
-      </c>
-      <c r="F3" t="s">
-        <v>21</v>
       </c>
       <c r="G3">
         <v>199158293</v>
@@ -687,33 +645,27 @@
         <v>723</v>
       </c>
       <c r="I3" t="s">
-        <v>16</v>
-      </c>
-      <c r="J3">
-        <v>0</v>
-      </c>
-      <c r="K3" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B4">
         <v>39667525772</v>
       </c>
       <c r="C4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" t="s">
+        <v>22</v>
+      </c>
+      <c r="F4" t="s">
         <v>23</v>
-      </c>
-      <c r="D4" t="s">
-        <v>19</v>
-      </c>
-      <c r="E4" t="s">
-        <v>24</v>
-      </c>
-      <c r="F4" t="s">
-        <v>25</v>
       </c>
       <c r="G4">
         <v>0</v>
@@ -722,33 +674,27 @@
         <v>705</v>
       </c>
       <c r="I4" t="s">
-        <v>16</v>
-      </c>
-      <c r="J4" t="s">
-        <v>56</v>
-      </c>
-      <c r="K4" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B5">
         <v>34153706524</v>
       </c>
       <c r="C5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" t="s">
+        <v>26</v>
+      </c>
+      <c r="F5" t="s">
         <v>27</v>
-      </c>
-      <c r="D5" t="s">
-        <v>19</v>
-      </c>
-      <c r="E5" t="s">
-        <v>28</v>
-      </c>
-      <c r="F5" t="s">
-        <v>29</v>
       </c>
       <c r="G5">
         <v>0</v>
@@ -757,33 +703,27 @@
         <v>690</v>
       </c>
       <c r="I5" t="s">
-        <v>30</v>
-      </c>
-      <c r="J5">
-        <v>33075000</v>
-      </c>
-      <c r="K5" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B6">
         <v>12646406653</v>
       </c>
       <c r="C6" t="s">
+        <v>30</v>
+      </c>
+      <c r="D6" t="s">
+        <v>17</v>
+      </c>
+      <c r="E6" t="s">
+        <v>31</v>
+      </c>
+      <c r="F6" t="s">
         <v>32</v>
-      </c>
-      <c r="D6" t="s">
-        <v>19</v>
-      </c>
-      <c r="E6" t="s">
-        <v>33</v>
-      </c>
-      <c r="F6" t="s">
-        <v>34</v>
       </c>
       <c r="G6">
         <v>0</v>
@@ -792,30 +732,24 @@
         <v>324</v>
       </c>
       <c r="I6" t="s">
-        <v>35</v>
-      </c>
-      <c r="J6">
-        <v>0</v>
-      </c>
-      <c r="K6" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B7">
         <v>64845344238</v>
       </c>
       <c r="C7" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D7" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E7" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="F7">
         <v>779971788</v>
@@ -827,30 +761,24 @@
         <v>607</v>
       </c>
       <c r="I7" t="s">
-        <v>39</v>
-      </c>
-      <c r="J7">
-        <v>16292519.6</v>
-      </c>
-      <c r="K7" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B8">
         <v>51345661305</v>
       </c>
       <c r="C8" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D8" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E8" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="F8">
         <v>790676752</v>
@@ -862,29 +790,23 @@
         <v>347</v>
       </c>
       <c r="I8" t="s">
-        <v>35</v>
-      </c>
-      <c r="J8" t="s">
-        <v>56</v>
-      </c>
-      <c r="K8" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B9">
         <v>37066501525</v>
       </c>
       <c r="C9" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D9" t="s">
-        <v>13</v>
-      </c>
-      <c r="E9" s="4">
+        <v>11</v>
+      </c>
+      <c r="E9" s="3">
         <v>36502</v>
       </c>
       <c r="F9">
@@ -897,29 +819,23 @@
         <v>614</v>
       </c>
       <c r="I9" t="s">
-        <v>39</v>
-      </c>
-      <c r="J9">
-        <v>7700000</v>
-      </c>
-      <c r="K9" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B10">
         <v>47037347674</v>
       </c>
       <c r="C10" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D10" t="s">
-        <v>13</v>
-      </c>
-      <c r="E10" s="4">
+        <v>11</v>
+      </c>
+      <c r="E10" s="3">
         <v>32761</v>
       </c>
       <c r="F10">
@@ -932,30 +848,24 @@
         <v>605</v>
       </c>
       <c r="I10" t="s">
-        <v>39</v>
-      </c>
-      <c r="J10">
-        <v>21000000</v>
-      </c>
-      <c r="K10" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B11">
         <v>96893291228</v>
       </c>
       <c r="C11" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D11" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E11" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="F11">
         <v>839733321</v>
@@ -967,30 +877,24 @@
         <v>762</v>
       </c>
       <c r="I11" t="s">
-        <v>50</v>
-      </c>
-      <c r="J11">
-        <v>41121469.655000001</v>
-      </c>
-      <c r="K11" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B12">
         <v>37083944036</v>
       </c>
       <c r="C12" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D12" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E12" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="F12">
         <v>952167725</v>
@@ -1002,13 +906,7 @@
         <v>694</v>
       </c>
       <c r="I12" t="s">
-        <v>30</v>
-      </c>
-      <c r="J12" t="s">
-        <v>56</v>
-      </c>
-      <c r="K12" t="s">
-        <v>57</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>